<commit_message>
Updated training objective for GitHub
</commit_message>
<xml_diff>
--- a/Project Planning/Skills Audit/Individual Skill Audit/Bijay Giri.xlsx
+++ b/Project Planning/Skills Audit/Individual Skill Audit/Bijay Giri.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Individual Skill Audit\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\L5\Semester-2\MANA541 - Project Management - 14805 - WIN - 201910\The-Clehuderfax-e-chain\Project Planning\Skills Audit\Individual Skill Audit\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{390699A4-172B-4182-9A9C-BE7E0BC4115D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DCD45BF6-15E9-4C4F-B35A-AD545E981029}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="1605" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -152,9 +152,6 @@
     <t>To become better manage communication, events and in tracking progress.</t>
   </si>
   <si>
-    <t>To become better at tools provided by GitHub for version control of our website.</t>
-  </si>
-  <si>
     <t>To develop prototype for user experience.</t>
   </si>
   <si>
@@ -213,6 +210,9 @@
   </si>
   <si>
     <t>Bijay Giri</t>
+  </si>
+  <si>
+    <t>To become better at tools provided by GitHub for version control and documentation of our website.</t>
   </si>
 </sst>
 </file>
@@ -1094,8 +1094,8 @@
   </sheetPr>
   <dimension ref="A1:I24"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
-      <selection activeCell="H7" sqref="H7:H24"/>
+    <sheetView tabSelected="1" topLeftCell="A18" workbookViewId="0">
+      <selection activeCell="E22" sqref="E22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1139,7 +1139,7 @@
       </c>
       <c r="C3" s="25"/>
       <c r="D3" s="20" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="E3" s="20" t="s">
         <v>1</v>
@@ -1211,7 +1211,7 @@
         <v>3</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E7" s="3" t="s">
         <v>26</v>
@@ -1223,7 +1223,7 @@
         <v>43891</v>
       </c>
       <c r="H7" s="11" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="I7" s="8"/>
     </row>
@@ -1238,7 +1238,7 @@
         <v>4</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E8" s="3" t="s">
         <v>25</v>
@@ -1250,7 +1250,7 @@
         <v>43891</v>
       </c>
       <c r="H8" s="11" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="I8" s="1"/>
     </row>
@@ -1265,7 +1265,7 @@
         <v>5</v>
       </c>
       <c r="D9" s="5" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E9" s="5" t="s">
         <v>27</v>
@@ -1277,7 +1277,7 @@
         <v>43891</v>
       </c>
       <c r="H9" s="11" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="I9" s="1"/>
     </row>
@@ -1292,7 +1292,7 @@
         <v>5</v>
       </c>
       <c r="D10" s="5" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="E10" s="5" t="s">
         <v>28</v>
@@ -1304,7 +1304,7 @@
         <v>43891</v>
       </c>
       <c r="H10" s="11" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="I10" s="1"/>
     </row>
@@ -1319,7 +1319,7 @@
         <v>5</v>
       </c>
       <c r="D11" s="5" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E11" s="5" t="s">
         <v>29</v>
@@ -1331,7 +1331,7 @@
         <v>43891</v>
       </c>
       <c r="H11" s="11" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="I11" s="1"/>
     </row>
@@ -1346,7 +1346,7 @@
         <v>4</v>
       </c>
       <c r="D12" s="5" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="E12" s="5" t="s">
         <v>31</v>
@@ -1358,7 +1358,7 @@
         <v>43898</v>
       </c>
       <c r="H12" s="11" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="I12" s="1"/>
     </row>
@@ -1373,7 +1373,7 @@
         <v>4</v>
       </c>
       <c r="D13" s="5" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E13" s="5" t="s">
         <v>30</v>
@@ -1385,7 +1385,7 @@
         <v>43898</v>
       </c>
       <c r="H13" s="11" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="I13" s="1"/>
     </row>
@@ -1400,7 +1400,7 @@
         <v>5</v>
       </c>
       <c r="D14" s="5" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E14" s="5" t="s">
         <v>32</v>
@@ -1412,7 +1412,7 @@
         <v>43891</v>
       </c>
       <c r="H14" s="11" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="I14" s="1"/>
     </row>
@@ -1427,7 +1427,7 @@
         <v>3</v>
       </c>
       <c r="D15" s="7" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="E15" s="7" t="s">
         <v>33</v>
@@ -1439,7 +1439,7 @@
         <v>43898</v>
       </c>
       <c r="H15" s="11" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="I15" s="1"/>
     </row>
@@ -1454,7 +1454,7 @@
         <v>4</v>
       </c>
       <c r="D16" s="7" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E16" s="7" t="s">
         <v>34</v>
@@ -1466,7 +1466,7 @@
         <v>43891</v>
       </c>
       <c r="H16" s="11" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="I16" s="1"/>
     </row>
@@ -1481,7 +1481,7 @@
         <v>3</v>
       </c>
       <c r="D17" s="13" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="E17" s="13" t="s">
         <v>38</v>
@@ -1493,7 +1493,7 @@
         <v>43898</v>
       </c>
       <c r="H17" s="11" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="18" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1507,10 +1507,10 @@
         <v>3</v>
       </c>
       <c r="D18" s="13" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E18" s="13" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="F18" s="12">
         <v>10</v>
@@ -1519,7 +1519,7 @@
         <v>43898</v>
       </c>
       <c r="H18" s="11" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="19" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1533,10 +1533,10 @@
         <v>3</v>
       </c>
       <c r="D19" s="13" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E19" s="13" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="F19" s="12">
         <v>3</v>
@@ -1545,7 +1545,7 @@
         <v>43891</v>
       </c>
       <c r="H19" s="11" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="20" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1559,10 +1559,10 @@
         <v>4</v>
       </c>
       <c r="D20" s="13" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="E20" s="13" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="F20" s="12">
         <v>3</v>
@@ -1571,7 +1571,7 @@
         <v>43891</v>
       </c>
       <c r="H20" s="11" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="21" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1585,7 +1585,7 @@
         <v>5</v>
       </c>
       <c r="D21" s="13" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="E21" s="13" t="s">
         <v>39</v>
@@ -1597,7 +1597,7 @@
         <v>43891</v>
       </c>
       <c r="H21" s="11" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="22" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1611,10 +1611,10 @@
         <v>3</v>
       </c>
       <c r="D22" s="13" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="E22" s="13" t="s">
-        <v>40</v>
+        <v>60</v>
       </c>
       <c r="F22" s="12">
         <v>3</v>
@@ -1623,7 +1623,7 @@
         <v>43891</v>
       </c>
       <c r="H22" s="11" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="23" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1637,10 +1637,10 @@
         <v>3</v>
       </c>
       <c r="D23" s="13" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="E23" s="13" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="F23" s="12">
         <v>10</v>
@@ -1649,7 +1649,7 @@
         <v>43898</v>
       </c>
       <c r="H23" s="11" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="24" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1657,16 +1657,16 @@
         <v>18</v>
       </c>
       <c r="B24" s="16" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C24" s="15">
         <v>4</v>
       </c>
       <c r="D24" s="16" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="E24" s="16" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="F24" s="15">
         <v>3</v>
@@ -1675,7 +1675,7 @@
         <v>43891</v>
       </c>
       <c r="H24" s="11" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated training hours and Team Skills Audit
</commit_message>
<xml_diff>
--- a/Project Planning/Skills Audit/Individual Skill Audit/Bijay Giri.xlsx
+++ b/Project Planning/Skills Audit/Individual Skill Audit/Bijay Giri.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\L5\Semester-2\MANA541 - Project Management - 14805 - WIN - 201910\The-Clehuderfax-e-chain\Project Planning\Skills Audit\Individual Skill Audit\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DCD45BF6-15E9-4C4F-B35A-AD545E981029}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{99152F67-6936-47DF-BC53-B7F21E5F34A2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="1605" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -1094,8 +1094,8 @@
   </sheetPr>
   <dimension ref="A1:I24"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A18" workbookViewId="0">
-      <selection activeCell="E22" sqref="E22"/>
+    <sheetView tabSelected="1" topLeftCell="A5" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1217,7 +1217,7 @@
         <v>26</v>
       </c>
       <c r="F7" s="4">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="G7" s="9">
         <v>43891</v>
@@ -1244,7 +1244,7 @@
         <v>25</v>
       </c>
       <c r="F8" s="4">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="G8" s="9">
         <v>43891</v>
@@ -1271,7 +1271,7 @@
         <v>27</v>
       </c>
       <c r="F9" s="4">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="G9" s="9">
         <v>43891</v>
@@ -1281,7 +1281,7 @@
       </c>
       <c r="I9" s="1"/>
     </row>
-    <row r="10" spans="1:9" ht="78.75" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9" ht="94.5" x14ac:dyDescent="0.25">
       <c r="A10" s="4">
         <v>4</v>
       </c>
@@ -1298,7 +1298,7 @@
         <v>28</v>
       </c>
       <c r="F10" s="4">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="G10" s="9">
         <v>43891</v>
@@ -1325,7 +1325,7 @@
         <v>29</v>
       </c>
       <c r="F11" s="4">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="G11" s="9">
         <v>43891</v>
@@ -1352,7 +1352,7 @@
         <v>31</v>
       </c>
       <c r="F12" s="4">
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="G12" s="9">
         <v>43898</v>
@@ -1379,7 +1379,7 @@
         <v>30</v>
       </c>
       <c r="F13" s="4">
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="G13" s="9">
         <v>43898</v>
@@ -1406,7 +1406,7 @@
         <v>32</v>
       </c>
       <c r="F14" s="4">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="G14" s="9">
         <v>43891</v>
@@ -1433,7 +1433,7 @@
         <v>33</v>
       </c>
       <c r="F15" s="6">
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="G15" s="9">
         <v>43898</v>
@@ -1460,7 +1460,7 @@
         <v>34</v>
       </c>
       <c r="F16" s="6">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="G16" s="9">
         <v>43891</v>
@@ -1486,8 +1486,8 @@
       <c r="E17" s="13" t="s">
         <v>38</v>
       </c>
-      <c r="F17" s="12">
-        <v>10</v>
+      <c r="F17" s="6">
+        <v>2</v>
       </c>
       <c r="G17" s="9">
         <v>43898</v>
@@ -1512,8 +1512,8 @@
       <c r="E18" s="13" t="s">
         <v>53</v>
       </c>
-      <c r="F18" s="12">
-        <v>10</v>
+      <c r="F18" s="6">
+        <v>2</v>
       </c>
       <c r="G18" s="9">
         <v>43898</v>
@@ -1538,8 +1538,8 @@
       <c r="E19" s="13" t="s">
         <v>55</v>
       </c>
-      <c r="F19" s="12">
-        <v>3</v>
+      <c r="F19" s="6">
+        <v>2</v>
       </c>
       <c r="G19" s="9">
         <v>43891</v>
@@ -1564,8 +1564,8 @@
       <c r="E20" s="13" t="s">
         <v>54</v>
       </c>
-      <c r="F20" s="12">
-        <v>3</v>
+      <c r="F20" s="6">
+        <v>2</v>
       </c>
       <c r="G20" s="9">
         <v>43891</v>
@@ -1591,7 +1591,7 @@
         <v>39</v>
       </c>
       <c r="F21" s="12">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="G21" s="9">
         <v>43891</v>
@@ -1617,7 +1617,7 @@
         <v>60</v>
       </c>
       <c r="F22" s="12">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="G22" s="9">
         <v>43891</v>
@@ -1643,7 +1643,7 @@
         <v>40</v>
       </c>
       <c r="F23" s="12">
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="G23" s="14">
         <v>43898</v>
@@ -1668,8 +1668,8 @@
       <c r="E24" s="16" t="s">
         <v>57</v>
       </c>
-      <c r="F24" s="15">
-        <v>3</v>
+      <c r="F24" s="12">
+        <v>2</v>
       </c>
       <c r="G24" s="17">
         <v>43891</v>

</xml_diff>